<commit_message>
q1a done 2a group by step1
</commit_message>
<xml_diff>
--- a/Q1/o1/a1.xlsx
+++ b/Q1/o1/a1.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\u\w\ecScala\w2\chapter4\o1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\u\w\ecScala\w2\scalding1\Q1\o1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,6 +17,9 @@
     <sheet name="Products" sheetId="4" r:id="rId3"/>
     <sheet name="prod after join 1" sheetId="2" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Products!$J$3:$J$33</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -27,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="115">
   <si>
     <t>primaryType_p1_reco</t>
   </si>
@@ -225,6 +228,153 @@
   </si>
   <si>
     <t>run_t2a_badminton</t>
+  </si>
+  <si>
+    <t>pId</t>
+  </si>
+  <si>
+    <t>c1</t>
+  </si>
+  <si>
+    <t>c2</t>
+  </si>
+  <si>
+    <t>c3</t>
+  </si>
+  <si>
+    <t>c2a</t>
+  </si>
+  <si>
+    <t>c2b</t>
+  </si>
+  <si>
+    <t>c2c</t>
+  </si>
+  <si>
+    <t>p9</t>
+  </si>
+  <si>
+    <t>p10</t>
+  </si>
+  <si>
+    <t>p11</t>
+  </si>
+  <si>
+    <t>office</t>
+  </si>
+  <si>
+    <t>black</t>
+  </si>
+  <si>
+    <t>p12</t>
+  </si>
+  <si>
+    <t>p13</t>
+  </si>
+  <si>
+    <t>elegant</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>p14</t>
+  </si>
+  <si>
+    <t>p15</t>
+  </si>
+  <si>
+    <t>p16</t>
+  </si>
+  <si>
+    <t>p17</t>
+  </si>
+  <si>
+    <t>p18</t>
+  </si>
+  <si>
+    <t>p19</t>
+  </si>
+  <si>
+    <t>p20</t>
+  </si>
+  <si>
+    <t>p21</t>
+  </si>
+  <si>
+    <t>p22</t>
+  </si>
+  <si>
+    <t>p23</t>
+  </si>
+  <si>
+    <t>p24</t>
+  </si>
+  <si>
+    <t>p25</t>
+  </si>
+  <si>
+    <t>p26</t>
+  </si>
+  <si>
+    <t>p27</t>
+  </si>
+  <si>
+    <t>p28</t>
+  </si>
+  <si>
+    <t>p29</t>
+  </si>
+  <si>
+    <t>p30</t>
+  </si>
+  <si>
+    <t>p31</t>
+  </si>
+  <si>
+    <t>_cat_full_formula</t>
+  </si>
+  <si>
+    <t>run_c2a_fast</t>
+  </si>
+  <si>
+    <t>jog_c2b_summer</t>
+  </si>
+  <si>
+    <t>run_c2a_tennis</t>
+  </si>
+  <si>
+    <t>walk_c2b_stroll</t>
+  </si>
+  <si>
+    <t>walk_c2c_saunter</t>
+  </si>
+  <si>
+    <t>jog_c2a_summer</t>
+  </si>
+  <si>
+    <t>run_c2b_tennis</t>
+  </si>
+  <si>
+    <t>run_c2a_badminton</t>
+  </si>
+  <si>
+    <t>walk_c2a_office</t>
+  </si>
+  <si>
+    <t>walk_elegant_office</t>
+  </si>
+  <si>
+    <t>jog_t2b_summer</t>
+  </si>
+  <si>
+    <t>run_t2a_tennis</t>
+  </si>
+  <si>
+    <t>walk_t2b_stroll</t>
+  </si>
+  <si>
+    <t>walk_t2c_saunter</t>
   </si>
 </sst>
 </file>
@@ -542,6 +692,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -645,6 +796,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:U9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1137,15 +1289,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H9"/>
+  <sheetPr codeName="Sheet3"/>
+  <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="A1:H9"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32:G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="8" max="8" width="17.85546875" customWidth="1"/>
+    <col min="10" max="10" width="21.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -1170,36 +1327,43 @@
       <c r="H1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I2" t="str">
+        <f>CONCATENATE(E2,"_",F2,"_",G2)</f>
+        <v>c1_c2_c3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>35</v>
-      </c>
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" t="s">
-        <v>59</v>
-      </c>
-      <c r="G2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>17</v>
       </c>
       <c r="B3" t="s">
         <v>18</v>
@@ -1208,82 +1372,133 @@
         <v>19</v>
       </c>
       <c r="D3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I3" t="str">
+        <f t="shared" ref="I3:J33" si="0">CONCATENATE(E3,"_",F3,"_",G3)</f>
+        <v>run_c2a_fast</v>
+      </c>
+      <c r="J3" t="s">
+        <v>101</v>
+      </c>
+      <c r="L3" t="s">
+        <v>81</v>
+      </c>
+      <c r="M3">
+        <v>14</v>
+      </c>
+      <c r="N3" t="str">
+        <f>CONCATENATE(L3,M3)</f>
+        <v>p14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
         <v>20</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E4" t="s">
         <v>4</v>
       </c>
-      <c r="F3" t="s">
-        <v>58</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="F4" t="s">
+        <v>71</v>
+      </c>
+      <c r="G4" t="s">
         <v>6</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="I4" t="str">
+        <f t="shared" si="0"/>
+        <v>jog_c2b_summer</v>
+      </c>
+      <c r="J4" t="s">
+        <v>106</v>
+      </c>
+      <c r="L4" t="s">
+        <v>81</v>
+      </c>
+      <c r="M4">
+        <v>15</v>
+      </c>
+      <c r="N4" t="str">
+        <f t="shared" ref="N4:N20" si="1">CONCATENATE(L4,M4)</f>
+        <v>p15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>37</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>23</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C5" t="s">
         <v>38</v>
       </c>
-      <c r="D4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" t="s">
         <v>11</v>
       </c>
-      <c r="F4" t="s">
-        <v>59</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="F5" t="s">
+        <v>70</v>
+      </c>
+      <c r="G5" t="s">
         <v>39</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H5" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="I5" t="str">
+        <f t="shared" si="0"/>
+        <v>run_c2a_tennis</v>
+      </c>
+      <c r="J5" t="s">
+        <v>106</v>
+      </c>
+      <c r="L5" t="s">
+        <v>81</v>
+      </c>
+      <c r="M5">
+        <v>16</v>
+      </c>
+      <c r="N5" t="str">
+        <f t="shared" si="1"/>
+        <v>p16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>48</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>42</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C6" t="s">
         <v>43</v>
-      </c>
-      <c r="D5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" t="s">
-        <v>49</v>
-      </c>
-      <c r="F5" t="s">
-        <v>58</v>
-      </c>
-      <c r="G5" t="s">
-        <v>50</v>
-      </c>
-      <c r="H5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" t="s">
-        <v>53</v>
       </c>
       <c r="D6" t="s">
         <v>24</v>
@@ -1292,76 +1507,127 @@
         <v>49</v>
       </c>
       <c r="F6" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="G6" t="s">
+        <v>50</v>
+      </c>
+      <c r="H6" t="s">
+        <v>47</v>
+      </c>
+      <c r="I6" t="str">
+        <f t="shared" si="0"/>
+        <v>walk_c2b_stroll</v>
+      </c>
+      <c r="J6" t="s">
+        <v>102</v>
+      </c>
+      <c r="L6" t="s">
+        <v>81</v>
+      </c>
+      <c r="M6">
+        <v>17</v>
+      </c>
+      <c r="N6" t="str">
+        <f t="shared" si="1"/>
+        <v>p17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" t="s">
+        <v>72</v>
+      </c>
+      <c r="G7" t="s">
         <v>55</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H7" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="I7" t="str">
+        <f t="shared" si="0"/>
+        <v>walk_c2c_saunter</v>
+      </c>
+      <c r="J7" t="s">
+        <v>111</v>
+      </c>
+      <c r="L7" t="s">
+        <v>81</v>
+      </c>
+      <c r="M7">
+        <v>18</v>
+      </c>
+      <c r="N7" t="str">
+        <f t="shared" si="1"/>
+        <v>p18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>22</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>23</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C8" t="s">
         <v>19</v>
       </c>
-      <c r="D7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="D8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" t="s">
         <v>4</v>
       </c>
-      <c r="F7" t="s">
-        <v>59</v>
-      </c>
-      <c r="G7" t="s">
+      <c r="F8" t="s">
+        <v>70</v>
+      </c>
+      <c r="G8" t="s">
         <v>6</v>
-      </c>
-      <c r="H7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>41</v>
-      </c>
-      <c r="B8" t="s">
-        <v>42</v>
-      </c>
-      <c r="C8" t="s">
-        <v>43</v>
-      </c>
-      <c r="D8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" t="s">
-        <v>58</v>
-      </c>
-      <c r="G8" t="s">
-        <v>39</v>
       </c>
       <c r="H8" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8" t="str">
+        <f t="shared" si="0"/>
+        <v>jog_c2a_summer</v>
+      </c>
+      <c r="J8" t="s">
+        <v>111</v>
+      </c>
+      <c r="L8" t="s">
+        <v>81</v>
+      </c>
+      <c r="M8">
+        <v>19</v>
+      </c>
+      <c r="N8" t="str">
+        <f t="shared" si="1"/>
+        <v>p19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B9" t="s">
         <v>42</v>
       </c>
       <c r="C9" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D9" t="s">
         <v>24</v>
@@ -1370,22 +1636,947 @@
         <v>11</v>
       </c>
       <c r="F9" t="s">
+        <v>71</v>
+      </c>
+      <c r="G9" t="s">
+        <v>39</v>
+      </c>
+      <c r="H9" t="s">
+        <v>25</v>
+      </c>
+      <c r="I9" t="str">
+        <f t="shared" si="0"/>
+        <v>run_c2b_tennis</v>
+      </c>
+      <c r="J9" t="s">
+        <v>111</v>
+      </c>
+      <c r="L9" t="s">
+        <v>81</v>
+      </c>
+      <c r="M9">
+        <v>20</v>
+      </c>
+      <c r="N9" t="str">
+        <f t="shared" si="1"/>
+        <v>p20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" t="s">
+        <v>70</v>
+      </c>
+      <c r="G10" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" t="s">
+        <v>47</v>
+      </c>
+      <c r="I10" t="str">
+        <f t="shared" si="0"/>
+        <v>run_c2a_badminton</v>
+      </c>
+      <c r="J10" t="s">
+        <v>111</v>
+      </c>
+      <c r="L10" t="s">
+        <v>81</v>
+      </c>
+      <c r="M10">
+        <v>21</v>
+      </c>
+      <c r="N10" t="str">
+        <f t="shared" si="1"/>
+        <v>p21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>73</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" t="s">
+        <v>70</v>
+      </c>
+      <c r="G11" t="s">
+        <v>6</v>
+      </c>
+      <c r="H11" t="s">
+        <v>25</v>
+      </c>
+      <c r="I11" t="str">
+        <f t="shared" si="0"/>
+        <v>jog_c2a_summer</v>
+      </c>
+      <c r="J11" t="s">
+        <v>108</v>
+      </c>
+      <c r="L11" t="s">
+        <v>81</v>
+      </c>
+      <c r="M11">
+        <v>22</v>
+      </c>
+      <c r="N11" t="str">
+        <f t="shared" si="1"/>
+        <v>p22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>74</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" t="s">
+        <v>70</v>
+      </c>
+      <c r="G12" t="s">
+        <v>15</v>
+      </c>
+      <c r="H12" t="s">
+        <v>25</v>
+      </c>
+      <c r="I12" t="str">
+        <f t="shared" si="0"/>
+        <v>run_c2a_badminton</v>
+      </c>
+      <c r="J12" t="s">
+        <v>108</v>
+      </c>
+      <c r="L12" t="s">
+        <v>81</v>
+      </c>
+      <c r="M12">
+        <v>23</v>
+      </c>
+      <c r="N12" t="str">
+        <f t="shared" si="1"/>
+        <v>p23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>75</v>
+      </c>
+      <c r="B13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" t="s">
+        <v>49</v>
+      </c>
+      <c r="F13" t="s">
+        <v>70</v>
+      </c>
+      <c r="G13" t="s">
+        <v>76</v>
+      </c>
+      <c r="H13" t="s">
+        <v>77</v>
+      </c>
+      <c r="I13" t="str">
+        <f t="shared" si="0"/>
+        <v>walk_c2a_office</v>
+      </c>
+      <c r="J13" t="s">
+        <v>101</v>
+      </c>
+      <c r="L13" t="s">
+        <v>81</v>
+      </c>
+      <c r="M13">
+        <v>24</v>
+      </c>
+      <c r="N13" t="str">
+        <f t="shared" si="1"/>
+        <v>p24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>78</v>
+      </c>
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" t="s">
+        <v>4</v>
+      </c>
+      <c r="F14" t="s">
+        <v>58</v>
+      </c>
+      <c r="G14" t="s">
+        <v>6</v>
+      </c>
+      <c r="H14" t="s">
+        <v>36</v>
+      </c>
+      <c r="I14" t="str">
+        <f t="shared" si="0"/>
+        <v>jog_t2b_summer</v>
+      </c>
+      <c r="J14" t="s">
+        <v>103</v>
+      </c>
+      <c r="L14" t="s">
+        <v>81</v>
+      </c>
+      <c r="M14">
+        <v>25</v>
+      </c>
+      <c r="N14" t="str">
+        <f t="shared" si="1"/>
+        <v>p25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>79</v>
+      </c>
+      <c r="B15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" t="s">
+        <v>49</v>
+      </c>
+      <c r="F15" t="s">
+        <v>80</v>
+      </c>
+      <c r="G15" t="s">
+        <v>76</v>
+      </c>
+      <c r="H15" t="s">
+        <v>77</v>
+      </c>
+      <c r="I15" t="str">
+        <f t="shared" si="0"/>
+        <v>walk_elegant_office</v>
+      </c>
+      <c r="J15" t="s">
+        <v>107</v>
+      </c>
+      <c r="L15" t="s">
+        <v>81</v>
+      </c>
+      <c r="M15">
+        <v>26</v>
+      </c>
+      <c r="N15" t="str">
+        <f t="shared" si="1"/>
+        <v>p26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>82</v>
+      </c>
+      <c r="B16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" t="s">
+        <v>49</v>
+      </c>
+      <c r="F16" t="s">
+        <v>60</v>
+      </c>
+      <c r="G16" t="s">
+        <v>55</v>
+      </c>
+      <c r="H16" t="s">
+        <v>21</v>
+      </c>
+      <c r="I16" t="str">
+        <f t="shared" si="0"/>
+        <v>walk_t2c_saunter</v>
+      </c>
+      <c r="J16" t="s">
+        <v>64</v>
+      </c>
+      <c r="L16" t="s">
+        <v>81</v>
+      </c>
+      <c r="M16">
+        <v>27</v>
+      </c>
+      <c r="N16" t="str">
+        <f t="shared" si="1"/>
+        <v>p27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>83</v>
+      </c>
+      <c r="B17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17" t="s">
+        <v>49</v>
+      </c>
+      <c r="F17" t="s">
+        <v>60</v>
+      </c>
+      <c r="G17" t="s">
+        <v>55</v>
+      </c>
+      <c r="H17" t="s">
+        <v>25</v>
+      </c>
+      <c r="I17" t="str">
+        <f t="shared" si="0"/>
+        <v>walk_t2c_saunter</v>
+      </c>
+      <c r="J17" t="s">
+        <v>64</v>
+      </c>
+      <c r="L17" t="s">
+        <v>81</v>
+      </c>
+      <c r="M17">
+        <v>28</v>
+      </c>
+      <c r="N17" t="str">
+        <f t="shared" si="1"/>
+        <v>p28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>84</v>
+      </c>
+      <c r="B18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" t="s">
+        <v>43</v>
+      </c>
+      <c r="D18" t="s">
+        <v>24</v>
+      </c>
+      <c r="E18" t="s">
+        <v>49</v>
+      </c>
+      <c r="F18" t="s">
+        <v>60</v>
+      </c>
+      <c r="G18" t="s">
+        <v>55</v>
+      </c>
+      <c r="H18" t="s">
+        <v>47</v>
+      </c>
+      <c r="I18" t="str">
+        <f t="shared" si="0"/>
+        <v>walk_t2c_saunter</v>
+      </c>
+      <c r="J18" t="s">
+        <v>112</v>
+      </c>
+      <c r="L18" t="s">
+        <v>81</v>
+      </c>
+      <c r="M18">
+        <v>29</v>
+      </c>
+      <c r="N18" t="str">
+        <f t="shared" si="1"/>
+        <v>p29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>85</v>
+      </c>
+      <c r="B19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" t="s">
+        <v>53</v>
+      </c>
+      <c r="D19" t="s">
+        <v>24</v>
+      </c>
+      <c r="E19" t="s">
+        <v>49</v>
+      </c>
+      <c r="F19" t="s">
+        <v>60</v>
+      </c>
+      <c r="G19" t="s">
+        <v>55</v>
+      </c>
+      <c r="H19" t="s">
+        <v>56</v>
+      </c>
+      <c r="I19" t="str">
+        <f t="shared" si="0"/>
+        <v>walk_t2c_saunter</v>
+      </c>
+      <c r="J19" t="s">
+        <v>112</v>
+      </c>
+      <c r="L19" t="s">
+        <v>81</v>
+      </c>
+      <c r="M19">
+        <v>30</v>
+      </c>
+      <c r="N19" t="str">
+        <f t="shared" si="1"/>
+        <v>p30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>86</v>
+      </c>
+      <c r="B20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20" t="s">
+        <v>24</v>
+      </c>
+      <c r="E20" t="s">
+        <v>4</v>
+      </c>
+      <c r="F20" t="s">
+        <v>58</v>
+      </c>
+      <c r="G20" t="s">
+        <v>6</v>
+      </c>
+      <c r="H20" t="s">
+        <v>36</v>
+      </c>
+      <c r="I20" t="str">
+        <f t="shared" si="0"/>
+        <v>jog_t2b_summer</v>
+      </c>
+      <c r="J20" t="s">
+        <v>112</v>
+      </c>
+      <c r="L20" t="s">
+        <v>81</v>
+      </c>
+      <c r="M20">
+        <v>31</v>
+      </c>
+      <c r="N20" t="str">
+        <f t="shared" si="1"/>
+        <v>p31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>87</v>
+      </c>
+      <c r="B21" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" t="s">
+        <v>20</v>
+      </c>
+      <c r="E21" t="s">
+        <v>4</v>
+      </c>
+      <c r="F21" t="s">
+        <v>58</v>
+      </c>
+      <c r="G21" t="s">
+        <v>6</v>
+      </c>
+      <c r="H21" t="s">
+        <v>21</v>
+      </c>
+      <c r="I21" t="str">
+        <f t="shared" si="0"/>
+        <v>jog_t2b_summer</v>
+      </c>
+      <c r="J21" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>88</v>
+      </c>
+      <c r="B22" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" t="s">
+        <v>24</v>
+      </c>
+      <c r="E22" t="s">
+        <v>11</v>
+      </c>
+      <c r="F22" t="s">
         <v>59</v>
       </c>
-      <c r="G9" t="s">
-        <v>15</v>
-      </c>
-      <c r="H9" t="s">
+      <c r="G22" t="s">
+        <v>39</v>
+      </c>
+      <c r="H22" t="s">
+        <v>25</v>
+      </c>
+      <c r="I22" t="str">
+        <f t="shared" si="0"/>
+        <v>run_t2a_tennis</v>
+      </c>
+      <c r="J22" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>89</v>
+      </c>
+      <c r="B23" t="s">
+        <v>42</v>
+      </c>
+      <c r="C23" t="s">
+        <v>43</v>
+      </c>
+      <c r="D23" t="s">
+        <v>24</v>
+      </c>
+      <c r="E23" t="s">
+        <v>49</v>
+      </c>
+      <c r="F23" t="s">
+        <v>58</v>
+      </c>
+      <c r="G23" t="s">
+        <v>50</v>
+      </c>
+      <c r="H23" t="s">
         <v>47</v>
       </c>
+      <c r="I23" t="str">
+        <f t="shared" si="0"/>
+        <v>walk_t2b_stroll</v>
+      </c>
+      <c r="J23" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>90</v>
+      </c>
+      <c r="B24" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" t="s">
+        <v>53</v>
+      </c>
+      <c r="D24" t="s">
+        <v>24</v>
+      </c>
+      <c r="E24" t="s">
+        <v>49</v>
+      </c>
+      <c r="F24" t="s">
+        <v>60</v>
+      </c>
+      <c r="G24" t="s">
+        <v>55</v>
+      </c>
+      <c r="H24" t="s">
+        <v>56</v>
+      </c>
+      <c r="I24" t="str">
+        <f t="shared" si="0"/>
+        <v>walk_t2c_saunter</v>
+      </c>
+      <c r="J24" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>91</v>
+      </c>
+      <c r="B25" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25" t="s">
+        <v>19</v>
+      </c>
+      <c r="D25" t="s">
+        <v>20</v>
+      </c>
+      <c r="E25" t="s">
+        <v>4</v>
+      </c>
+      <c r="F25" t="s">
+        <v>58</v>
+      </c>
+      <c r="G25" t="s">
+        <v>6</v>
+      </c>
+      <c r="H25" t="s">
+        <v>21</v>
+      </c>
+      <c r="I25" t="str">
+        <f t="shared" si="0"/>
+        <v>jog_t2b_summer</v>
+      </c>
+      <c r="J25" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>92</v>
+      </c>
+      <c r="B26" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" t="s">
+        <v>38</v>
+      </c>
+      <c r="D26" t="s">
+        <v>24</v>
+      </c>
+      <c r="E26" t="s">
+        <v>11</v>
+      </c>
+      <c r="F26" t="s">
+        <v>59</v>
+      </c>
+      <c r="G26" t="s">
+        <v>39</v>
+      </c>
+      <c r="H26" t="s">
+        <v>25</v>
+      </c>
+      <c r="I26" t="str">
+        <f t="shared" si="0"/>
+        <v>run_t2a_tennis</v>
+      </c>
+      <c r="J26" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>93</v>
+      </c>
+      <c r="B27" t="s">
+        <v>42</v>
+      </c>
+      <c r="C27" t="s">
+        <v>43</v>
+      </c>
+      <c r="D27" t="s">
+        <v>24</v>
+      </c>
+      <c r="E27" t="s">
+        <v>49</v>
+      </c>
+      <c r="F27" t="s">
+        <v>58</v>
+      </c>
+      <c r="G27" t="s">
+        <v>50</v>
+      </c>
+      <c r="H27" t="s">
+        <v>47</v>
+      </c>
+      <c r="I27" t="str">
+        <f t="shared" si="0"/>
+        <v>walk_t2b_stroll</v>
+      </c>
+      <c r="J27" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>94</v>
+      </c>
+      <c r="B28" t="s">
+        <v>18</v>
+      </c>
+      <c r="C28" t="s">
+        <v>53</v>
+      </c>
+      <c r="D28" t="s">
+        <v>24</v>
+      </c>
+      <c r="E28" t="s">
+        <v>4</v>
+      </c>
+      <c r="F28" t="s">
+        <v>58</v>
+      </c>
+      <c r="G28" t="s">
+        <v>6</v>
+      </c>
+      <c r="H28" t="s">
+        <v>56</v>
+      </c>
+      <c r="I28" t="str">
+        <f t="shared" si="0"/>
+        <v>jog_t2b_summer</v>
+      </c>
+      <c r="J28" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>95</v>
+      </c>
+      <c r="B29" t="s">
+        <v>18</v>
+      </c>
+      <c r="C29" t="s">
+        <v>19</v>
+      </c>
+      <c r="D29" t="s">
+        <v>24</v>
+      </c>
+      <c r="E29" t="s">
+        <v>11</v>
+      </c>
+      <c r="F29" t="s">
+        <v>59</v>
+      </c>
+      <c r="G29" t="s">
+        <v>12</v>
+      </c>
+      <c r="H29" t="s">
+        <v>36</v>
+      </c>
+      <c r="I29" t="str">
+        <f t="shared" si="0"/>
+        <v>run_t2a_fast</v>
+      </c>
+      <c r="J29" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>96</v>
+      </c>
+      <c r="B30" t="s">
+        <v>18</v>
+      </c>
+      <c r="C30" t="s">
+        <v>19</v>
+      </c>
+      <c r="D30" t="s">
+        <v>20</v>
+      </c>
+      <c r="E30" t="s">
+        <v>4</v>
+      </c>
+      <c r="F30" t="s">
+        <v>58</v>
+      </c>
+      <c r="G30" t="s">
+        <v>6</v>
+      </c>
+      <c r="H30" t="s">
+        <v>21</v>
+      </c>
+      <c r="I30" t="str">
+        <f t="shared" si="0"/>
+        <v>jog_t2b_summer</v>
+      </c>
+      <c r="J30" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>97</v>
+      </c>
+      <c r="B31" t="s">
+        <v>23</v>
+      </c>
+      <c r="C31" t="s">
+        <v>38</v>
+      </c>
+      <c r="D31" t="s">
+        <v>24</v>
+      </c>
+      <c r="E31" t="s">
+        <v>11</v>
+      </c>
+      <c r="F31" t="s">
+        <v>59</v>
+      </c>
+      <c r="G31" t="s">
+        <v>39</v>
+      </c>
+      <c r="H31" t="s">
+        <v>25</v>
+      </c>
+      <c r="I31" t="str">
+        <f t="shared" si="0"/>
+        <v>run_t2a_tennis</v>
+      </c>
+      <c r="J31" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>98</v>
+      </c>
+      <c r="B32" t="s">
+        <v>42</v>
+      </c>
+      <c r="C32" t="s">
+        <v>43</v>
+      </c>
+      <c r="D32" t="s">
+        <v>24</v>
+      </c>
+      <c r="E32" t="s">
+        <v>4</v>
+      </c>
+      <c r="F32" t="s">
+        <v>58</v>
+      </c>
+      <c r="G32" t="s">
+        <v>6</v>
+      </c>
+      <c r="H32" t="s">
+        <v>47</v>
+      </c>
+      <c r="I32" t="str">
+        <f t="shared" si="0"/>
+        <v>jog_t2b_summer</v>
+      </c>
+      <c r="J32" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>99</v>
+      </c>
+      <c r="B33" t="s">
+        <v>18</v>
+      </c>
+      <c r="C33" t="s">
+        <v>53</v>
+      </c>
+      <c r="D33" t="s">
+        <v>24</v>
+      </c>
+      <c r="E33" t="s">
+        <v>49</v>
+      </c>
+      <c r="F33" t="s">
+        <v>60</v>
+      </c>
+      <c r="G33" t="s">
+        <v>55</v>
+      </c>
+      <c r="H33" t="s">
+        <v>56</v>
+      </c>
+      <c r="I33" t="str">
+        <f t="shared" si="0"/>
+        <v>walk_t2c_saunter</v>
+      </c>
+      <c r="J33" t="s">
+        <v>114</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="J3:J33">
+    <sortState ref="J4:J33">
+      <sortCondition ref="J4:J33"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>